<commit_message>
matrix sizes are defined
</commit_message>
<xml_diff>
--- a/docs/Parameter Optimization/Parameter optimization.xlsx
+++ b/docs/Parameter Optimization/Parameter optimization.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5772"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,10 +365,13 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -392,192 +395,147 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>2593</v>
+        <v>2048</v>
       </c>
       <c r="B2" s="1">
         <v>256</v>
       </c>
       <c r="C2" s="1">
-        <f>((B2)^(0.5))/A2</f>
-        <v>6.1704589278827613E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D2" s="1">
-        <v>189.9</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="E2" s="1">
-        <v>201.4</v>
+        <v>89</v>
       </c>
       <c r="F2" s="1">
-        <v>257.8</v>
+        <v>101.1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>2591</v>
+        <v>2048</v>
       </c>
       <c r="B3" s="1">
         <v>256</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C10" si="0">((B3)^(0.5))/A3</f>
-        <v>6.1752219220378235E-3</v>
+        <v>2.8E-3</v>
       </c>
       <c r="D3" s="1">
-        <v>189.9</v>
+        <v>128.30000000000001</v>
       </c>
       <c r="E3" s="1">
-        <v>201.4</v>
+        <v>137.80000000000001</v>
       </c>
       <c r="F3" s="1">
-        <v>257.8</v>
+        <v>165.6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2617</v>
+        <v>2048</v>
       </c>
       <c r="B4" s="1">
         <v>256</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" si="0"/>
-        <v>6.1138708444784104E-3</v>
+        <v>1.2699999999999999E-2</v>
       </c>
       <c r="D4" s="1">
-        <v>189.2</v>
+        <v>256.5</v>
       </c>
       <c r="E4" s="1">
-        <v>201.4</v>
+        <v>269.2</v>
       </c>
       <c r="F4" s="1">
-        <v>230.2</v>
+        <v>294.39999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>2609</v>
+        <v>1024</v>
       </c>
       <c r="B5" s="1">
         <v>256</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="0"/>
-        <v>6.1326178612495213E-3</v>
+        <v>3.9999999999999998E-7</v>
       </c>
       <c r="D5" s="1">
-        <v>189.9</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="E5" s="1">
-        <v>201.4</v>
+        <v>88.1</v>
       </c>
       <c r="F5" s="1">
-        <v>257.8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>2677</v>
+        <v>1024</v>
       </c>
       <c r="B6" s="1">
         <v>256</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="0"/>
-        <v>5.9768397459843111E-3</v>
+        <v>3.3000000000000002E-6</v>
       </c>
       <c r="D6" s="1">
-        <v>188.5</v>
+        <v>128.69999999999999</v>
       </c>
       <c r="E6" s="1">
-        <v>200.1</v>
+        <v>138.80000000000001</v>
       </c>
       <c r="F6" s="1">
-        <v>255.7</v>
+        <v>141.19999999999999</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>2693</v>
+        <v>1024</v>
       </c>
       <c r="B7" s="1">
         <v>256</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>5.9413293724470849E-3</v>
+        <v>5.1999999999999997E-5</v>
       </c>
       <c r="D7" s="1">
-        <v>187.9</v>
+        <v>256.8</v>
       </c>
       <c r="E7" s="1">
-        <v>199.4</v>
+        <v>275.5</v>
       </c>
       <c r="F7" s="1">
-        <v>230.2</v>
+        <v>272.8</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>3001</v>
-      </c>
-      <c r="B8" s="1">
-        <v>256</v>
-      </c>
-      <c r="C8" s="1">
-        <f t="shared" si="0"/>
-        <v>5.3315561479506833E-3</v>
-      </c>
-      <c r="D8" s="1">
-        <v>182.5</v>
-      </c>
-      <c r="E8" s="1">
-        <v>194.1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>230.2</v>
-      </c>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>2903</v>
-      </c>
-      <c r="B9" s="1">
-        <v>256</v>
-      </c>
-      <c r="C9" s="1">
-        <f t="shared" si="0"/>
-        <v>5.5115397864278336E-3</v>
-      </c>
-      <c r="D9" s="1">
-        <v>183.9</v>
-      </c>
-      <c r="E9" s="1">
-        <v>196.7</v>
-      </c>
-      <c r="F9" s="1">
-        <v>230.2</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>2833</v>
-      </c>
-      <c r="B10" s="1">
-        <v>256</v>
-      </c>
-      <c r="C10" s="1">
-        <f t="shared" si="0"/>
-        <v>5.6477232615601836E-3</v>
-      </c>
-      <c r="D10" s="1">
-        <v>185.2</v>
-      </c>
-      <c r="E10" s="1">
-        <v>198.1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>230.2</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D12" s="1">

</xml_diff>

<commit_message>
codes for benchmark testing and benchmark values are updated
</commit_message>
<xml_diff>
--- a/docs/Parameter Optimization/Parameter optimization.xlsx
+++ b/docs/Parameter Optimization/Parameter optimization.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>q</t>
   </si>
@@ -42,6 +42,30 @@
   </si>
   <si>
     <t>dual</t>
+  </si>
+  <si>
+    <t>plain text size(bytes)</t>
+  </si>
+  <si>
+    <t>private key size (bytes)</t>
+  </si>
+  <si>
+    <t>public key size (bytes)</t>
+  </si>
+  <si>
+    <t>cipher text size (bytes)</t>
+  </si>
+  <si>
+    <t>cipher text size(AES encrypted) (bytes)</t>
+  </si>
+  <si>
+    <t>key generation time (s)</t>
+  </si>
+  <si>
+    <t>encryption time (s)</t>
+  </si>
+  <si>
+    <t>decryption time (s)</t>
   </si>
 </sst>
 </file>
@@ -77,9 +101,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -97,6 +124,221 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>41148</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Right Brace 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16139160" y="198120"/>
+          <a:ext cx="277368" cy="1234440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>48768</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Right Brace 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16146780" y="2964180"/>
+          <a:ext cx="277368" cy="1234440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="28575"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-IN" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="968022" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16588740" y="693420"/>
+          <a:ext cx="968022" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Regev system</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="881716" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16603980" y="3467100"/>
+          <a:ext cx="881716" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-IN" sz="1100"/>
+            <a:t>Dual system</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -362,18 +604,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="19.5546875" customWidth="1"/>
+    <col min="9" max="9" width="23.109375" customWidth="1"/>
+    <col min="10" max="10" width="20.88671875" customWidth="1"/>
+    <col min="11" max="11" width="21.77734375" customWidth="1"/>
+    <col min="12" max="12" width="32.5546875" customWidth="1"/>
+    <col min="13" max="13" width="17.109375" customWidth="1"/>
+    <col min="14" max="14" width="18.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -392,8 +642,32 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>2048</v>
       </c>
@@ -412,8 +686,32 @@
       <c r="F2" s="1">
         <v>101.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G2" s="1">
+        <v>48</v>
+      </c>
+      <c r="H2" s="2">
+        <v>4016</v>
+      </c>
+      <c r="I2" s="1">
+        <v>0.107054</v>
+      </c>
+      <c r="J2" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K2" s="2">
+        <v>263168</v>
+      </c>
+      <c r="L2" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1.3061</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0.70121299999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2048</v>
       </c>
@@ -432,8 +730,32 @@
       <c r="F3" s="1">
         <v>165.6</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G3" s="1">
+        <v>48</v>
+      </c>
+      <c r="H3" s="2">
+        <v>4016</v>
+      </c>
+      <c r="I3" s="1">
+        <v>9.9258600000000002E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K3" s="2">
+        <v>263168</v>
+      </c>
+      <c r="L3" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M3" s="1">
+        <v>1.3409899999999999</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0.74512599999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2048</v>
       </c>
@@ -452,28 +774,48 @@
       <c r="F4" s="1">
         <v>294.39999999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>1024</v>
-      </c>
-      <c r="B5" s="1">
-        <v>256</v>
-      </c>
-      <c r="C5" s="1">
-        <v>3.9999999999999998E-7</v>
-      </c>
-      <c r="D5" s="1">
-        <v>81.900000000000006</v>
-      </c>
-      <c r="E5" s="1">
-        <v>88.1</v>
-      </c>
-      <c r="F5" s="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" s="1">
+        <v>48</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4016</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0.10073</v>
+      </c>
+      <c r="J4" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K4" s="1">
+        <v>263168</v>
+      </c>
+      <c r="L4" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M4" s="1">
+        <v>1.3602700000000001</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0.78195000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1024</v>
       </c>
@@ -481,19 +823,43 @@
         <v>256</v>
       </c>
       <c r="C6" s="1">
-        <v>3.3000000000000002E-6</v>
+        <v>3.9999999999999998E-7</v>
       </c>
       <c r="D6" s="1">
-        <v>128.69999999999999</v>
+        <v>81.900000000000006</v>
       </c>
       <c r="E6" s="1">
-        <v>138.80000000000001</v>
+        <v>88.1</v>
       </c>
       <c r="F6" s="1">
-        <v>141.19999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="G6" s="1">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4016</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.101601</v>
+      </c>
+      <c r="J6" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K6" s="1">
+        <v>263168</v>
+      </c>
+      <c r="L6" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M6" s="1">
+        <v>1.3008299999999999</v>
+      </c>
+      <c r="N6" s="1">
+        <v>0.715673</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>1024</v>
       </c>
@@ -501,76 +867,496 @@
         <v>256</v>
       </c>
       <c r="C7" s="1">
+        <v>3.3000000000000002E-6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>128.69999999999999</v>
+      </c>
+      <c r="E7" s="1">
+        <v>138.80000000000001</v>
+      </c>
+      <c r="F7" s="1">
+        <v>141.19999999999999</v>
+      </c>
+      <c r="G7" s="1">
+        <v>48</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4016</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0.101128</v>
+      </c>
+      <c r="J7" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K7" s="1">
+        <v>263168</v>
+      </c>
+      <c r="L7" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M7" s="1">
+        <v>1.3042499999999999</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0.69264899999999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B8" s="1">
+        <v>256</v>
+      </c>
+      <c r="C8" s="1">
         <v>5.1999999999999997E-5</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D8" s="1">
         <v>256.8</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E8" s="1">
         <v>275.5</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F8" s="1">
         <v>272.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G8" s="1">
+        <v>48</v>
+      </c>
+      <c r="H8" s="1">
+        <v>4016</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.100494</v>
+      </c>
+      <c r="J8" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K8" s="1">
+        <v>263168</v>
+      </c>
+      <c r="L8" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M8" s="1">
+        <v>1.30593</v>
+      </c>
+      <c r="N8" s="1">
+        <v>0.68488499999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D12" s="1">
-        <v>80</v>
-      </c>
-      <c r="E12" s="1">
-        <v>100</v>
-      </c>
-      <c r="F12" s="1">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="1">
-        <v>128</v>
-      </c>
-      <c r="E13" s="1">
-        <v>170</v>
-      </c>
-      <c r="F13" s="1">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="1">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>2048</v>
+      </c>
+      <c r="B17" s="1">
         <v>256</v>
       </c>
-      <c r="E14" s="1">
-        <v>300</v>
-      </c>
-      <c r="F14" s="1">
-        <v>350</v>
+      <c r="C17" s="1">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="D17" s="1">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="E17" s="1">
+        <v>89</v>
+      </c>
+      <c r="F17" s="1">
+        <v>101.1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>48</v>
+      </c>
+      <c r="H17" s="2">
+        <v>262160</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0.93189500000000003</v>
+      </c>
+      <c r="J17" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K17" s="2">
+        <v>5024</v>
+      </c>
+      <c r="L17" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M17" s="1">
+        <v>0.73505799999999999</v>
+      </c>
+      <c r="N17" s="1">
+        <v>0.701793</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>2048</v>
+      </c>
+      <c r="B18" s="1">
+        <v>256</v>
+      </c>
+      <c r="C18" s="1">
+        <v>2.8E-3</v>
+      </c>
+      <c r="D18" s="1">
+        <v>128.30000000000001</v>
+      </c>
+      <c r="E18" s="1">
+        <v>137.80000000000001</v>
+      </c>
+      <c r="F18" s="1">
+        <v>165.6</v>
+      </c>
+      <c r="G18" s="1">
+        <v>48</v>
+      </c>
+      <c r="H18" s="1">
+        <v>262160</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0.90437900000000004</v>
+      </c>
+      <c r="J18" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K18" s="1">
+        <v>5024</v>
+      </c>
+      <c r="L18" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.76141999999999999</v>
+      </c>
+      <c r="N18" s="1">
+        <v>0.74290100000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>2048</v>
+      </c>
+      <c r="B19" s="1">
+        <v>256</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>256.5</v>
+      </c>
+      <c r="E19" s="1">
+        <v>269.2</v>
+      </c>
+      <c r="F19" s="1">
+        <v>294.39999999999998</v>
+      </c>
+      <c r="G19" s="1">
+        <v>48</v>
+      </c>
+      <c r="H19" s="1">
+        <v>262160</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0.92392200000000002</v>
+      </c>
+      <c r="J19" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K19" s="1">
+        <v>5024</v>
+      </c>
+      <c r="L19" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M19" s="1">
+        <v>0.80472900000000003</v>
+      </c>
+      <c r="N19" s="1">
+        <v>0.70699699999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B21" s="1">
+        <v>256</v>
+      </c>
+      <c r="C21" s="1">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="D21" s="1">
+        <v>81.900000000000006</v>
+      </c>
+      <c r="E21" s="1">
+        <v>88.1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>91</v>
+      </c>
+      <c r="G21" s="1">
+        <v>48</v>
+      </c>
+      <c r="H21" s="2">
+        <v>262160</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.90729099999999996</v>
+      </c>
+      <c r="J21" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K21" s="1">
+        <v>5024</v>
+      </c>
+      <c r="L21" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M21" s="1">
+        <v>0.80529600000000001</v>
+      </c>
+      <c r="N21" s="1">
+        <v>0.75619199999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B22" s="1">
+        <v>256</v>
+      </c>
+      <c r="C22" s="1">
+        <v>3.3000000000000002E-6</v>
+      </c>
+      <c r="D22" s="1">
+        <v>128.69999999999999</v>
+      </c>
+      <c r="E22" s="1">
+        <v>138.80000000000001</v>
+      </c>
+      <c r="F22" s="1">
+        <v>141.19999999999999</v>
+      </c>
+      <c r="G22" s="1">
+        <v>48</v>
+      </c>
+      <c r="H22" s="1">
+        <v>262160</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0.91962699999999997</v>
+      </c>
+      <c r="J22" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K22" s="1">
+        <v>5024</v>
+      </c>
+      <c r="L22" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.82543299999999997</v>
+      </c>
+      <c r="N22" s="1">
+        <v>0.73463800000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B23" s="1">
+        <v>256</v>
+      </c>
+      <c r="C23" s="1">
+        <v>5.1999999999999997E-5</v>
+      </c>
+      <c r="D23" s="1">
+        <v>256.8</v>
+      </c>
+      <c r="E23" s="1">
+        <v>275.5</v>
+      </c>
+      <c r="F23" s="1">
+        <v>272.8</v>
+      </c>
+      <c r="G23" s="1">
+        <v>48</v>
+      </c>
+      <c r="H23" s="1">
+        <v>262160</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0.92376499999999995</v>
+      </c>
+      <c r="J23" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="K23" s="1">
+        <v>5024</v>
+      </c>
+      <c r="L23" s="2">
+        <v>4367517</v>
+      </c>
+      <c r="M23" s="1">
+        <v>0.80065399999999998</v>
+      </c>
+      <c r="N23" s="1">
+        <v>0.76468499999999995</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>